<commit_message>
updated CR_210_2 pub index and rebuilt
</commit_message>
<xml_diff>
--- a/publication/part1000/CR_210_2/Bugzilla_list.xlsx
+++ b/publication/part1000/CR_210_2/Bugzilla_list.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klt/Projets/EclipseWS/stepmod/publication/part1000/CR_210_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klt/Projets/EclipseWS/stepmod/publication/part1000/CR_210_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="15480"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -1596,13 +1596,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:M149" totalsRowShown="0" headerRowDxfId="19">
-  <autoFilter ref="A1:M149">
-    <filterColumn colId="6">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:M149"/>
   <tableColumns count="13">
     <tableColumn id="1" name="Type" dataDxfId="18"/>
     <tableColumn id="5" name="Type Text" dataDxfId="17"/>
@@ -1929,22 +1923,22 @@
   <dimension ref="A1:M149"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L74" sqref="L74"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="4" customWidth="1"/>
     <col min="2" max="2" width="21.33203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="17.5" style="4" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="29.6640625" style="19" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" style="19" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" style="7" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="4" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" style="19" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" style="19" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" style="7" customWidth="1"/>
     <col min="7" max="7" width="35.1640625" style="19" customWidth="1"/>
-    <col min="8" max="8" width="5.6640625" style="4" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="7.1640625" style="4" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="7.6640625" style="4" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="5.6640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="7.1640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="7.6640625" style="4" customWidth="1"/>
     <col min="11" max="11" width="14.5" style="4" customWidth="1"/>
     <col min="12" max="12" width="100.33203125" style="2" customWidth="1"/>
     <col min="13" max="13" width="10.1640625" style="2" customWidth="1"/>
@@ -1992,7 +1986,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:13" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2014,7 +2008,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:13" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2036,7 +2030,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="4" spans="1:13" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2058,7 +2052,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:13" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2080,7 +2074,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:13" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2100,7 +2094,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="7" spans="1:13" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2124,7 +2118,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:13" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2146,7 +2140,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:13" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2168,7 +2162,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:13" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>0</v>
       </c>
@@ -2190,7 +2184,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:13" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -2214,7 +2208,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:13" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>0</v>
       </c>
@@ -2236,7 +2230,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:13" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>0</v>
       </c>
@@ -2258,7 +2252,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:13" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -2280,7 +2274,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:13" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>0</v>
       </c>
@@ -2302,7 +2296,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:13" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -2324,7 +2318,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>0</v>
       </c>
@@ -2346,7 +2340,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
@@ -2370,7 +2364,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
@@ -2392,7 +2386,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>156</v>
       </c>
@@ -2416,7 +2410,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
@@ -2438,7 +2432,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>4</v>
       </c>
@@ -2462,7 +2456,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>4</v>
       </c>
@@ -2484,7 +2478,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>0</v>
       </c>
@@ -2506,7 +2500,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>0</v>
       </c>
@@ -2528,7 +2522,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>0</v>
       </c>
@@ -2550,7 +2544,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>0</v>
       </c>
@@ -2574,7 +2568,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>0</v>
       </c>
@@ -2596,7 +2590,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>0</v>
       </c>
@@ -2642,7 +2636,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>0</v>
       </c>
@@ -2664,7 +2658,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>4</v>
       </c>
@@ -2688,7 +2682,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
@@ -2712,7 +2706,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
@@ -2734,7 +2728,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>7</v>
       </c>
@@ -2756,7 +2750,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>0</v>
       </c>
@@ -2778,7 +2772,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>7</v>
       </c>
@@ -2800,7 +2794,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>4</v>
       </c>
@@ -2824,7 +2818,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>4</v>
       </c>
@@ -2848,7 +2842,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>3</v>
       </c>
@@ -2872,7 +2866,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>4</v>
       </c>
@@ -2896,7 +2890,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>7</v>
       </c>
@@ -2918,7 +2912,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>7</v>
       </c>
@@ -2940,7 +2934,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>0</v>
       </c>
@@ -2994,7 +2988,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>0</v>
       </c>
@@ -3016,7 +3010,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>3</v>
       </c>
@@ -3040,7 +3034,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>7</v>
       </c>
@@ -3062,7 +3056,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>3</v>
       </c>
@@ -3086,7 +3080,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>3</v>
       </c>
@@ -3110,7 +3104,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="5">
         <v>3</v>
       </c>
@@ -3135,7 +3129,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="52" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>0</v>
       </c>
@@ -3189,7 +3183,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="54" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>3</v>
       </c>
@@ -3211,7 +3205,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="55" spans="1:12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>3</v>
       </c>
@@ -3261,7 +3255,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="57" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>3</v>
       </c>
@@ -3285,7 +3279,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="58" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>3</v>
       </c>
@@ -3309,7 +3303,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="59" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>3</v>
       </c>
@@ -3359,7 +3353,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="61" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>3</v>
       </c>
@@ -3383,7 +3377,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>0</v>
       </c>
@@ -3405,7 +3399,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="63" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>3</v>
       </c>
@@ -3429,7 +3423,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="64" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>8</v>
       </c>
@@ -3451,7 +3445,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="65" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>0</v>
       </c>
@@ -3473,7 +3467,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="66" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>3</v>
       </c>
@@ -3497,7 +3491,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="67" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>3</v>
       </c>
@@ -3521,7 +3515,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="68" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>3</v>
       </c>
@@ -3545,7 +3539,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="69" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>3</v>
       </c>
@@ -3569,7 +3563,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="70" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>3</v>
       </c>
@@ -3593,7 +3587,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="71" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>4</v>
       </c>
@@ -3617,7 +3611,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="72" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>3</v>
       </c>
@@ -3671,7 +3665,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="96" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" ht="64" x14ac:dyDescent="0.2">
       <c r="A74" s="5">
         <v>3</v>
       </c>
@@ -3700,7 +3694,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="75" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>3</v>
       </c>
@@ -3752,7 +3746,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="77" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>6</v>
       </c>
@@ -3774,7 +3768,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="78" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>6</v>
       </c>
@@ -3796,7 +3790,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="79" spans="1:12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>3</v>
       </c>
@@ -3824,7 +3818,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="80" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>2</v>
       </c>
@@ -3848,7 +3842,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="81" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>3</v>
       </c>
@@ -3872,7 +3866,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="82" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>3</v>
       </c>
@@ -3896,7 +3890,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="83" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>0</v>
       </c>
@@ -3918,7 +3912,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="84" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>0</v>
       </c>
@@ -3940,7 +3934,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="85" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>0</v>
       </c>
@@ -3962,7 +3956,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="86" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>3</v>
       </c>
@@ -3986,7 +3980,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="87" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>0</v>
       </c>
@@ -4010,7 +4004,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="88" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>0</v>
       </c>
@@ -4032,7 +4026,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="89" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>0</v>
       </c>
@@ -4056,7 +4050,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="90" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>7</v>
       </c>
@@ -4078,7 +4072,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="91" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>7</v>
       </c>
@@ -4100,7 +4094,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="92" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>7</v>
       </c>
@@ -4122,7 +4116,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="93" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>3</v>
       </c>
@@ -4182,7 +4176,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="95" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>158</v>
       </c>
@@ -4206,7 +4200,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="96" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>3</v>
       </c>
@@ -4230,7 +4224,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="97" spans="1:13" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>0</v>
       </c>
@@ -4252,7 +4246,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="98" spans="1:13" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>0</v>
       </c>
@@ -4274,7 +4268,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="99" spans="1:13" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>0</v>
       </c>
@@ -4296,7 +4290,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="100" spans="1:13" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>3</v>
       </c>
@@ -4322,7 +4316,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="101" spans="1:13" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>3</v>
       </c>
@@ -4374,7 +4368,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="103" spans="1:13" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>3</v>
       </c>
@@ -4398,7 +4392,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="104" spans="1:13" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>0</v>
       </c>
@@ -4423,7 +4417,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:13" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>3</v>
       </c>
@@ -4447,7 +4441,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="106" spans="1:13" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>3</v>
       </c>
@@ -4471,7 +4465,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="107" spans="1:13" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>3</v>
       </c>
@@ -4495,7 +4489,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="108" spans="1:13" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>3</v>
       </c>
@@ -4519,7 +4513,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="109" spans="1:13" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="5">
         <v>3</v>
       </c>
@@ -4542,7 +4536,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="110" spans="1:13" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>3</v>
       </c>
@@ -4566,7 +4560,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="111" spans="1:13" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>4</v>
       </c>
@@ -4612,7 +4606,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="113" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>4</v>
       </c>
@@ -4634,7 +4628,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="114" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>3</v>
       </c>
@@ -4658,7 +4652,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="115" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>3</v>
       </c>
@@ -4682,7 +4676,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="116" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>13</v>
       </c>
@@ -4704,7 +4698,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="117" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>3</v>
       </c>
@@ -4728,7 +4722,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="118" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>3</v>
       </c>
@@ -4752,7 +4746,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="119" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>3</v>
       </c>
@@ -4776,7 +4770,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="120" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>3</v>
       </c>
@@ -4800,7 +4794,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="121" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>0</v>
       </c>
@@ -4822,7 +4816,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="122" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>3</v>
       </c>
@@ -4846,7 +4840,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="123" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>3</v>
       </c>
@@ -4870,7 +4864,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="124" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>3</v>
       </c>
@@ -4894,7 +4888,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="125" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>3</v>
       </c>
@@ -4918,7 +4912,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="126" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A126" s="5">
         <v>3</v>
       </c>
@@ -5008,7 +5002,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="129" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>13</v>
       </c>
@@ -5030,7 +5024,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="130" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>13</v>
       </c>
@@ -5052,7 +5046,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="131" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>13</v>
       </c>
@@ -5074,7 +5068,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="132" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>13</v>
       </c>
@@ -5096,7 +5090,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="133" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>13</v>
       </c>
@@ -5118,7 +5112,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="134" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>13</v>
       </c>
@@ -5140,7 +5134,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="135" spans="1:12" customFormat="1" ht="17.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:12" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>13</v>
       </c>
@@ -5170,7 +5164,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="136" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>13</v>
       </c>
@@ -5216,7 +5210,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="138" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>3</v>
       </c>
@@ -5238,7 +5232,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="139" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>3</v>
       </c>
@@ -5286,7 +5280,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="141" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>3</v>
       </c>
@@ -5310,7 +5304,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="142" spans="1:12" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>3</v>
       </c>
@@ -5358,7 +5352,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="144" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -5402,7 +5396,7 @@
       </c>
       <c r="M145" s="12"/>
     </row>
-    <row r="146" spans="1:13" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A146" s="8"/>
       <c r="B146" s="8"/>
       <c r="C146" s="8"/>
@@ -5463,7 +5457,7 @@
       </c>
       <c r="M148" s="12"/>
     </row>
-    <row r="149" spans="1:13" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A149" s="8"/>
       <c r="B149" s="8"/>
       <c r="C149" s="8"/>

</xml_diff>